<commit_message>
Added copy as PDF
</commit_message>
<xml_diff>
--- a/Rechnungen/Berechnungen-Master.xlsx
+++ b/Rechnungen/Berechnungen-Master.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Massdata\Magellan2\LeapData\Desktop\Projects\CarbonbindingForestsWorldWide\Rechnungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5240CDB-A8D4-480D-8FBD-4ED11EFDB542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798175A9-7E31-4536-A19B-1DCAC6892BEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rechnungen" sheetId="1" r:id="rId1"/>
-    <sheet name="Quellen" sheetId="2" r:id="rId2"/>
+    <sheet name="Anmerkungen" sheetId="3" r:id="rId2"/>
+    <sheet name="Quellen" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Berechnungen für die Speicherkraft von Wäldern im Bereich des Kohlenstoffes</t>
   </si>
@@ -180,13 +181,76 @@
     <t>Forstart</t>
   </si>
   <si>
-    <t>Kohlenstoffspeicherung:</t>
-  </si>
-  <si>
     <t>Kohlenstoffspeicherung pro Hektar</t>
   </si>
   <si>
     <t>CO2-Bindung pro Hektar Wald</t>
+  </si>
+  <si>
+    <t>https://www.holzistgenial.at/blog/1-kubikmeter-holz-bindet-1-tonne-co2/</t>
+  </si>
+  <si>
+    <t>https://www.ndr.de/ratgeber/klimawandel/CO2-Speicher-Wie-wird-der-Wald-fit-fuer-den-Klimawandel,wald994.html</t>
+  </si>
+  <si>
+    <t>https://www.baysf.de/de/wald-verstehen/wald-kohlendioxid.html</t>
+  </si>
+  <si>
+    <t>Alle Quellen abgerufen am 09.04.2021</t>
+  </si>
+  <si>
+    <t>Datenquellen, sortiert nach erscheinen in den Rechnungen:</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>Quellen</t>
+  </si>
+  <si>
+    <t>7./8./9.</t>
+  </si>
+  <si>
+    <t>Anmerkungen zu den Rechnungen</t>
+  </si>
+  <si>
+    <t>Werte unterliegen jährlichen schwankungen (ich gehe von ca. 10% aus)</t>
+  </si>
+  <si>
+    <t>Die Kohlenstoff-Speicherung insgesammt bezieht sich auf einen ausgewachsenen Hektar Wald, neu absorbiert werden in einem Wald pro Hektar p.a. rund 10-12 Tonnen neues CO2</t>
+  </si>
+  <si>
+    <t>Die Korreturfaktoren sind je nach Literaturquelle unterschiedlich bemessen</t>
+  </si>
+  <si>
+    <t>Es wird keine Garantie auf Richtigkeit der Rechnungen übernommen, wenngleich diese mit bestem Wissen und Gewissen erstellt wurden</t>
+  </si>
+  <si>
+    <t>Die Datenquellen (grade für den Regenwald) sind von sehr unterschiedlicher Qualität</t>
+  </si>
+  <si>
+    <t>Kohlenstoffberechnungen</t>
+  </si>
+  <si>
+    <t>Der subtropische Regenwald inkludiert auch zu Teilen wüstenähnliche Gebiete, deshalb ist dieser Wert niedriger als erwartet.</t>
   </si>
 </sst>
 </file>
@@ -206,7 +270,7 @@
     <numFmt numFmtId="179" formatCode="0.00\ &quot;Tonnen C&quot;"/>
     <numFmt numFmtId="180" formatCode="0.00\ &quot;Tonnen CO2&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +301,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -255,11 +333,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -274,8 +356,11 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -662,13 +747,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
@@ -678,60 +763,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -765,23 +870,23 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>700</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <f>C8/4.5</f>
         <v>155.55555555555554</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>42</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>1.2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <f>G8*1.6</f>
         <v>0.92799999999999994</v>
       </c>
@@ -790,23 +895,23 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>375</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <f>C9/3</f>
         <v>125</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>35</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
         <v>0.53800000000000003</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <f t="shared" ref="H9:H11" si="0">G9*1.6</f>
         <v>0.86080000000000012</v>
       </c>
@@ -815,23 +920,23 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>410</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="11">
         <f>C10/2</f>
         <v>205</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>30</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="7">
         <v>0.75</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="4">
         <v>0.6</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
@@ -840,23 +945,23 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>835</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="11">
         <f>C11/3.2</f>
         <v>260.9375</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <v>32</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="7">
         <v>0.88</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="4">
         <v>0.52</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>0.83200000000000007</v>
       </c>
@@ -891,180 +996,191 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <f>((F8/4)^2*3.1415)*E8*0.8</f>
         <v>9.4998960000000015</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <f>C17*(H8*1000)</f>
         <v>8815.9034879999999</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <f>D17/1000</f>
         <v>8.815903488</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="10">
         <f>D8*C17</f>
         <v>1477.7616</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="9">
         <f>E17*D8</f>
         <v>1371.3627647999999</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <f>((F9/4)^2*3.1415)*E9*0.8</f>
         <v>5.4976250000000002</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <f t="shared" ref="D18:D20" si="1">C18*(H9*1000)</f>
         <v>4732.3556000000008</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <f t="shared" ref="E18:E20" si="2">D18/1000</f>
         <v>4.7323556000000009</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="10">
         <f t="shared" ref="F18:F20" si="3">D9*C18</f>
         <v>687.203125</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="9">
         <f t="shared" ref="G18:G20" si="4">E18*D9</f>
         <v>591.5444500000001</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <f>((F10/4)^2*3.1415)*E10*0.8</f>
         <v>2.6506406250000003</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <f t="shared" si="1"/>
         <v>2544.6150000000002</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <f t="shared" si="2"/>
         <v>2.5446150000000003</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="10">
         <f t="shared" si="3"/>
         <v>543.3813281250001</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="9">
         <f t="shared" si="4"/>
         <v>521.64607500000011</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <f>((F11/4)^2*3.1415)*E11*0.8</f>
         <v>3.8924441600000002</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <f t="shared" si="1"/>
         <v>3238.5135411200004</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <f t="shared" si="2"/>
         <v>3.2385135411200006</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="10">
         <f t="shared" si="3"/>
         <v>1015.684648</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="9">
         <f t="shared" si="4"/>
         <v>845.04962713600014</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>25</v>
       </c>
       <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="12">
         <f>G17*0.25</f>
         <v>342.84069119999998</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="13">
         <f>C29*3.67</f>
         <v>1258.2253367039998</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="12">
         <f>G18*0.25</f>
         <v>147.88611250000002</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="13">
         <f t="shared" ref="D30:D32" si="5">C30*3.67</f>
         <v>542.74203287500006</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="12">
         <f>G19*0.25</f>
         <v>130.41151875000003</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="13">
         <f t="shared" si="5"/>
         <v>478.61027381250011</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="12">
         <f>G20*0.25</f>
         <v>211.26240678400004</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="13">
         <f t="shared" si="5"/>
         <v>775.33303289728008</v>
       </c>
@@ -1084,36 +1200,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BD0D8D-6C70-4224-8CFE-8C3B88887C65}">
-  <dimension ref="B7:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8E861C7-04B8-4E93-A332-E12D8C33BA29}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BD0D8D-6C70-4224-8CFE-8C3B88887C65}">
+  <dimension ref="A5:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{DF18CC88-F8E2-4BD2-89A8-149585247B39}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{282719DA-4C58-412F-925A-A34D99399EEE}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{11A912BD-16C7-4B28-9DCA-8660E17A92DF}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{AF20D486-FF0C-4D27-B82A-953CA54D23E4}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{16CFF151-26FF-499D-9256-A239DF57F909}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>